<commit_message>
filters back in, salmonella filter update
</commit_message>
<xml_diff>
--- a/dependencies/bi/salmonella/heidelberg-SL476/script_dependents/DefiningSNPsGroupDesignations.xlsx
+++ b/dependencies/bi/salmonella/heidelberg-SL476/script_dependents/DefiningSNPsGroupDesignations.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Grouping</t>
   </si>
@@ -54,6 +54,12 @@
   </si>
   <si>
     <t>NC_011083.1-2751478</t>
+  </si>
+  <si>
+    <t>NC_011083.1-602044</t>
+  </si>
+  <si>
+    <t>heidelberg-03</t>
   </si>
 </sst>
 </file>
@@ -1139,8 +1145,12 @@
       </c>
     </row>
     <row r="6" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="6"/>
-      <c r="B6"/>
+      <c r="A6" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7"/>

</xml_diff>